<commit_message>
Correct system layer design table
</commit_message>
<xml_diff>
--- a/doc/System layers.xlsx
+++ b/doc/System layers.xlsx
@@ -23,9 +23,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>EnigmaIoT</t>
-  </si>
-  <si>
     <t>ESP-NOW</t>
   </si>
   <si>
@@ -33,9 +30,6 @@
   </si>
   <si>
     <t>nRF24F1</t>
-  </si>
-  <si>
-    <t>443MHz</t>
   </si>
   <si>
     <t>CayenneLPP</t>
@@ -46,12 +40,18 @@
   <si>
     <t>Encription (ChaCha20, Speck+CFB, AES+CFB)</t>
   </si>
+  <si>
+    <t>EnigmaIoT Protocol</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -170,6 +170,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -233,24 +240,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -259,6 +248,21 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="2" tint="0.39994506668294322"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="0" tint="-0.249977111117893"/>
       </patternFill>
     </fill>
   </fills>
@@ -572,10 +576,10 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -584,37 +588,37 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1193,7 +1197,7 @@
   <dimension ref="F14:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1204,46 +1208,46 @@
     <row r="17" spans="6:10" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="6:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F18" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="6:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F19" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="9"/>
     </row>
     <row r="20" spans="6:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="6:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="10"/>
-    </row>
-    <row r="21" spans="6:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="11" t="s">
+      <c r="G21" s="2"/>
+      <c r="H21" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13" t="s">
+      <c r="I21" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I21" s="14" t="s">
-        <v>3</v>
-      </c>
       <c r="J21" s="15" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>